<commit_message>
Updates to L05 assignment and slides
</commit_message>
<xml_diff>
--- a/docs/materials/Labs/L05-A-Interpreter.xlsx
+++ b/docs/materials/Labs/L05-A-Interpreter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/braught/courses/Spring23/COMP256/website/docs/old_materials/labs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/braught/courses/Spring23/COMP256/website/docs/materials/Labs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB80DD4B-FC94-504A-9D34-1235C917FF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55669D05-371A-3E40-AB67-89E31231F5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="-19740" windowWidth="27640" windowHeight="16940" xr2:uid="{BC79AE93-6DDC-984D-B6ED-C5270FAF6D21}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{BC79AE93-6DDC-984D-B6ED-C5270FAF6D21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>A positive (1234) or negative (-1234) integer value.</t>
   </si>
   <si>
-    <t>A line label.  Must be a string of capital letters or digits.</t>
-  </si>
-  <si>
     <t>A variable.  Must be a single letter.</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>Displays a ? as a prompt and reads an integer value from standard input into a variable.</t>
+  </si>
+  <si>
+    <t>A line label.  Must be a string of capital letters.</t>
   </si>
 </sst>
 </file>
@@ -868,7 +868,7 @@
   <dimension ref="F5:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -897,12 +897,12 @@
     </row>
     <row r="7" spans="6:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="7"/>
       <c r="I7" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="6:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -916,7 +916,7 @@
         <v>18</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="6:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -927,10 +927,10 @@
         <v>9</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="6:12" ht="52" customHeight="1" x14ac:dyDescent="0.2">
@@ -941,10 +941,10 @@
         <v>10</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="6:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -955,7 +955,7 @@
         <v>11</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>12</v>
@@ -969,10 +969,10 @@
         <v>13</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="6:12" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -986,13 +986,13 @@
         <v>15</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="6:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="6:12" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L15" s="24" t="s">
         <v>3</v>
@@ -1003,7 +1003,7 @@
         <v>19</v>
       </c>
       <c r="L16" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="11:12" x14ac:dyDescent="0.2">
@@ -1019,7 +1019,7 @@
         <v>21</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="11:12" x14ac:dyDescent="0.2">
@@ -1027,7 +1027,7 @@
         <v>22</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="11:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1035,7 +1035,7 @@
         <v>23</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>